<commit_message>
1)Json -> xlsx 2)Clean code
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Id</t>
   </si>
@@ -30,6 +30,42 @@
   </si>
   <si>
     <t>Сумма</t>
+  </si>
+  <si>
+    <t>0000006274</t>
+  </si>
+  <si>
+    <t>Крем-борщ вегетарианский</t>
+  </si>
+  <si>
+    <t>0000006273</t>
+  </si>
+  <si>
+    <t>Окрошка на квасе</t>
+  </si>
+  <si>
+    <t>0000006255</t>
+  </si>
+  <si>
+    <t>Оливье с курой</t>
+  </si>
+  <si>
+    <t>0000002843</t>
+  </si>
+  <si>
+    <t>Рис с курицей в кисло-сладком соусе</t>
+  </si>
+  <si>
+    <t>0000006260</t>
+  </si>
+  <si>
+    <t>Бефстроганов с жареным картофелем и грибами</t>
+  </si>
+  <si>
+    <t>0000002878</t>
+  </si>
+  <si>
+    <t>SWEETBOX чиа-манго</t>
   </si>
 </sst>
 </file>
@@ -380,7 +416,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="E1" sqref="E1"/>
@@ -407,10 +443,104 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>47323424</v>
-      </c>
-      <c r="B2">
-        <v>47323424</v>
+        <v>357469</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>357470</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>357471</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>357473</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>357477</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>357478</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>